<commit_message>
updated arduino file to use level switches to make sure ball valves shut off if the level switch is activated
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Need to put level switch visuals on processor page</t>
   </si>
@@ -33,13 +33,16 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Solution\</t>
-  </si>
-  <si>
     <t>Need to verify that ball valves will operate from processor sketch</t>
   </si>
   <si>
     <t xml:space="preserve">Need to figure out why the old arduino board died. </t>
+  </si>
+  <si>
+    <t>Integrated, 9/23/19</t>
+  </si>
+  <si>
+    <t>Solution</t>
   </si>
 </sst>
 </file>
@@ -387,13 +390,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -404,12 +408,12 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>30948</v>
+        <v>30947</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -420,6 +424,9 @@
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -428,18 +435,20 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A2:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>